<commit_message>
new versions labor05 included
</commit_message>
<xml_diff>
--- a/parser-old/labor05/David_Quantenmusik.xlsx
+++ b/parser-old/labor05/David_Quantenmusik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanneswalter/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanneswalter/Dropbox/David_Cern/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83356D09-80A2-D14E-8A29-6427A6972ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E891499-A781-424D-A42A-C1F1FBB47FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55400" yWindow="-520" windowWidth="28800" windowHeight="17540" xr2:uid="{A8ECE7E4-C49A-964A-8521-062E1103D4BC}"/>
+    <workbookView xWindow="30660" yWindow="2640" windowWidth="28800" windowHeight="17540" xr2:uid="{A8ECE7E4-C49A-964A-8521-062E1103D4BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>g13</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>ja</t>
-  </si>
-  <si>
-    <t>(nicht benutzt..)</t>
   </si>
 </sst>
 </file>
@@ -573,7 +570,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,8 +765,8 @@
         <f>$E$1+(LOG(25/18,2)*1200)</f>
         <v>933.61742599889476</v>
       </c>
-      <c r="D12" t="s">
-        <v>56</v>
+      <c r="E12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>